<commit_message>
Updated ITA_grids model - 2025-09-02 13:11
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/SuppXLS/Scen_Par-AR6_R10.xlsx
+++ b/VerveStacks_ITA_grids/SuppXLS/Scen_Par-AR6_R10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439E1E32-6C23-47E0-A877-0B3E5DE2076D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DF7FC5-D9E9-4C64-AE9A-B33ADD577238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Veda" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="118">
   <si>
     <t>~Inputcell: 1-5</t>
   </si>
@@ -748,22 +748,22 @@
                   <c:v>325.04000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>341.29200000000003</c:v>
+                  <c:v>334.7912</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>380.29680000000002</c:v>
+                  <c:v>386.79759999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>429.05280000000005</c:v>
+                  <c:v>464.80720000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>487.56000000000006</c:v>
+                  <c:v>536.31600000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>546.06720000000007</c:v>
+                  <c:v>588.32240000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>588.32240000000002</c:v>
+                  <c:v>627.32720000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1039,19 +1039,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.48</c:v>
+                  <c:v>241.69</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>104.42</c:v>
+                  <c:v>339.03</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>134.85</c:v>
+                  <c:v>410.28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>178.1</c:v>
+                  <c:v>494.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>209.45</c:v>
+                  <c:v>635.42999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5642,9 +5642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AA61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -5677,7 +5675,7 @@
       </c>
       <c r="C5" s="1" t="str">
         <f>VLOOKUP(B3,$A$7:$C$999,3,FALSE)</f>
-        <v>C3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.45">
@@ -5701,8 +5699,9 @@
       <c r="B8" t="s">
         <v>105</v>
       </c>
-      <c r="C8" t="s">
-        <v>3</v>
+      <c r="C8" t="str">
+        <f>C7</f>
+        <v>C1</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
@@ -5718,8 +5717,9 @@
       <c r="B9" t="s">
         <v>106</v>
       </c>
-      <c r="C9" t="s">
-        <v>6</v>
+      <c r="C9" t="str">
+        <f t="shared" ref="C9:C61" si="0">C8</f>
+        <v>C1</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -5735,8 +5735,9 @@
       <c r="B10" t="s">
         <v>107</v>
       </c>
-      <c r="C10" t="s">
-        <v>8</v>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>C1</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -5756,8 +5757,9 @@
       <c r="B11" t="s">
         <v>108</v>
       </c>
-      <c r="C11" t="s">
-        <v>10</v>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>C1</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
@@ -5771,8 +5773,8 @@
         <v>109</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" ref="C9:C61" si="0">C11</f>
-        <v>C7</v>
+        <f t="shared" si="0"/>
+        <v>C1</v>
       </c>
       <c r="R12" s="8">
         <f>Q10</f>
@@ -5780,27 +5782,27 @@
       </c>
       <c r="S12" s="8">
         <f t="shared" ref="S12:X12" si="1">$Q$10*H13</f>
-        <v>341.29200000000003</v>
+        <v>334.7912</v>
       </c>
       <c r="T12" s="8">
         <f t="shared" si="1"/>
-        <v>380.29680000000002</v>
+        <v>386.79759999999999</v>
       </c>
       <c r="U12" s="8">
         <f t="shared" si="1"/>
-        <v>429.05280000000005</v>
+        <v>464.80720000000002</v>
       </c>
       <c r="V12" s="8">
         <f t="shared" si="1"/>
-        <v>487.56000000000006</v>
+        <v>536.31600000000003</v>
       </c>
       <c r="W12" s="8">
         <f t="shared" si="1"/>
-        <v>546.06720000000007</v>
+        <v>588.32240000000002</v>
       </c>
       <c r="X12" s="8">
         <f t="shared" si="1"/>
-        <v>588.32240000000002</v>
+        <v>627.32720000000006</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.45">
@@ -5812,7 +5814,7 @@
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>C7</v>
+        <v>C1</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -5823,27 +5825,27 @@
       </c>
       <c r="H13" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!H$15,ar6_r10!$M$2:$M$999,Veda!$E13)</f>
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="I13" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!I$15,ar6_r10!$M$2:$M$999,Veda!$E13)</f>
-        <v>1.17</v>
+        <v>1.19</v>
       </c>
       <c r="J13" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!J$15,ar6_r10!$M$2:$M$999,Veda!$E13)</f>
-        <v>1.32</v>
+        <v>1.43</v>
       </c>
       <c r="K13" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!K$15,ar6_r10!$M$2:$M$999,Veda!$E13)</f>
-        <v>1.5</v>
+        <v>1.65</v>
       </c>
       <c r="L13" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!L$15,ar6_r10!$M$2:$M$999,Veda!$E13)</f>
-        <v>1.68</v>
+        <v>1.81</v>
       </c>
       <c r="M13" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!M$15,ar6_r10!$M$2:$M$999,Veda!$E13)</f>
-        <v>1.81</v>
+        <v>1.93</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="17.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
@@ -5855,7 +5857,7 @@
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>C7</v>
+        <v>C1</v>
       </c>
       <c r="Q14" s="5" t="s">
         <v>13</v>
@@ -5870,7 +5872,7 @@
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>C7</v>
+        <v>C1</v>
       </c>
       <c r="G15" s="7">
         <v>2020</v>
@@ -5936,18 +5938,18 @@
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>C7</v>
+        <v>C1</v>
       </c>
       <c r="E16" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!G$15,ar6_r10!$M$2:$M$999,Veda!$E16)</f>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H16" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!H$15,ar6_r10!$M$2:$M$999,Veda!$E16)</f>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="I16" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!I$15,ar6_r10!$M$2:$M$999,Veda!$E16)</f>
@@ -5955,50 +5957,50 @@
       </c>
       <c r="J16" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!J$15,ar6_r10!$M$2:$M$999,Veda!$E16)</f>
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="K16" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!K$15,ar6_r10!$M$2:$M$999,Veda!$E16)</f>
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="L16" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!L$15,ar6_r10!$M$2:$M$999,Veda!$E16)</f>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="M16" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!M$15,ar6_r10!$M$2:$M$999,Veda!$E16)</f>
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="Q16" s="10" t="s">
         <v>17</v>
       </c>
       <c r="R16" s="6">
         <f t="shared" ref="R16:X18" si="3">G16*R$12</f>
-        <v>0</v>
+        <v>3.2504000000000004</v>
       </c>
       <c r="S16" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.347912</v>
       </c>
       <c r="T16" s="6">
         <f t="shared" si="3"/>
-        <v>3.8029680000000003</v>
+        <v>3.8679760000000001</v>
       </c>
       <c r="U16" s="6">
         <f t="shared" si="3"/>
-        <v>4.290528000000001</v>
+        <v>13.944216000000001</v>
       </c>
       <c r="V16" s="6">
         <f t="shared" si="3"/>
-        <v>4.8756000000000004</v>
+        <v>16.089480000000002</v>
       </c>
       <c r="W16" s="6">
         <f t="shared" si="3"/>
-        <v>10.921344000000001</v>
+        <v>23.532896000000001</v>
       </c>
       <c r="X16" s="6">
         <f t="shared" si="3"/>
-        <v>17.649671999999999</v>
+        <v>31.366360000000004</v>
       </c>
       <c r="Y16" t="s">
         <v>18</v>
@@ -6014,14 +6016,14 @@
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>C7</v>
+        <v>C1</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
       </c>
       <c r="G17" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!G$15,ar6_r10!$M$2:$M$999,Veda!$E17)</f>
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
       <c r="H17" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!H$15,ar6_r10!$M$2:$M$999,Veda!$E17)</f>
@@ -6029,7 +6031,7 @@
       </c>
       <c r="I17" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!I$15,ar6_r10!$M$2:$M$999,Veda!$E17)</f>
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="J17" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!J$15,ar6_r10!$M$2:$M$999,Veda!$E17)</f>
@@ -6041,42 +6043,42 @@
       </c>
       <c r="L17" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!L$15,ar6_r10!$M$2:$M$999,Veda!$E17)</f>
-        <v>0.28999999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="M17" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!M$15,ar6_r10!$M$2:$M$999,Veda!$E17)</f>
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="Q17" s="10" t="s">
         <v>20</v>
       </c>
       <c r="R17" s="6">
         <f t="shared" si="3"/>
-        <v>117.01440000000001</v>
+        <v>113.764</v>
       </c>
       <c r="S17" s="6">
         <f t="shared" si="3"/>
-        <v>109.21344000000001</v>
+        <v>107.133184</v>
       </c>
       <c r="T17" s="6">
         <f t="shared" si="3"/>
-        <v>117.892008</v>
+        <v>116.03927999999999</v>
       </c>
       <c r="U17" s="6">
         <f t="shared" si="3"/>
-        <v>124.42531200000001</v>
+        <v>134.79408799999999</v>
       </c>
       <c r="V17" s="6">
         <f t="shared" si="3"/>
-        <v>141.39240000000001</v>
+        <v>155.53164000000001</v>
       </c>
       <c r="W17" s="6">
         <f t="shared" si="3"/>
-        <v>158.359488</v>
+        <v>176.49672000000001</v>
       </c>
       <c r="X17" s="6">
         <f t="shared" si="3"/>
-        <v>176.49672000000001</v>
+        <v>194.47143200000002</v>
       </c>
       <c r="Y17" t="s">
         <v>18</v>
@@ -6098,19 +6100,19 @@
       </c>
       <c r="G18" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!G$15,ar6_r10!$M$2:$M$999,Veda!$E18)</f>
-        <v>0.6</v>
+        <v>0.61</v>
       </c>
       <c r="H18" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!H$15,ar6_r10!$M$2:$M$999,Veda!$E18)</f>
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="I18" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!I$15,ar6_r10!$M$2:$M$999,Veda!$E18)</f>
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="J18" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!J$15,ar6_r10!$M$2:$M$999,Veda!$E18)</f>
-        <v>0.56999999999999995</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="K18" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!K$15,ar6_r10!$M$2:$M$999,Veda!$E18)</f>
@@ -6118,7 +6120,7 @@
       </c>
       <c r="L18" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!L$15,ar6_r10!$M$2:$M$999,Veda!$E18)</f>
-        <v>0.52</v>
+        <v>0.53</v>
       </c>
       <c r="M18" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!M$15,ar6_r10!$M$2:$M$999,Veda!$E18)</f>
@@ -6129,31 +6131,31 @@
       </c>
       <c r="R18" s="6">
         <f t="shared" si="3"/>
-        <v>195.024</v>
+        <v>198.27440000000001</v>
       </c>
       <c r="S18" s="6">
         <f t="shared" si="3"/>
-        <v>204.77520000000001</v>
+        <v>207.57054400000001</v>
       </c>
       <c r="T18" s="6">
         <f t="shared" si="3"/>
-        <v>228.17807999999999</v>
+        <v>228.21058399999998</v>
       </c>
       <c r="U18" s="6">
         <f t="shared" si="3"/>
-        <v>244.56009600000002</v>
+        <v>260.29203200000006</v>
       </c>
       <c r="V18" s="6">
         <f t="shared" si="3"/>
-        <v>263.28240000000005</v>
+        <v>289.61064000000005</v>
       </c>
       <c r="W18" s="6">
         <f t="shared" si="3"/>
-        <v>283.95494400000007</v>
+        <v>311.81087200000002</v>
       </c>
       <c r="X18" s="6">
         <f t="shared" si="3"/>
-        <v>311.81087200000002</v>
+        <v>332.48341600000003</v>
       </c>
       <c r="Y18" t="s">
         <v>18</v>
@@ -6184,23 +6186,23 @@
       </c>
       <c r="I19" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!I$15,ar6_r10!$M$2:$M$999,Veda!$E19)</f>
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="J19" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!J$15,ar6_r10!$M$2:$M$999,Veda!$E19)</f>
-        <v>0.11</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K19" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!K$15,ar6_r10!$M$2:$M$999,Veda!$E19)</f>
-        <v>0.12</v>
+        <v>0.17</v>
       </c>
       <c r="L19" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!L$15,ar6_r10!$M$2:$M$999,Veda!$E19)</f>
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="M19" s="11">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!M$15,ar6_r10!$M$2:$M$999,Veda!$E19)</f>
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="Q19" s="10" t="s">
         <v>25</v>
@@ -6261,27 +6263,27 @@
       </c>
       <c r="S20" s="6">
         <f t="shared" si="6"/>
-        <v>17.552160000000015</v>
+        <v>10.336272000000008</v>
       </c>
       <c r="T20" s="6">
         <f t="shared" si="6"/>
-        <v>24.475512000000037</v>
+        <v>32.796536000000003</v>
       </c>
       <c r="U20" s="6">
         <f t="shared" si="6"/>
-        <v>50.316192000000058</v>
+        <v>59.969879999999989</v>
       </c>
       <c r="V20" s="6">
         <f t="shared" si="6"/>
-        <v>73.134000000000015</v>
+        <v>81.42252000000002</v>
       </c>
       <c r="W20" s="6">
         <f t="shared" si="6"/>
-        <v>94.00156800000002</v>
+        <v>90.263608000000033</v>
       </c>
       <c r="X20" s="6">
         <f t="shared" si="6"/>
-        <v>90.263608000000033</v>
+        <v>90.621151999999938</v>
       </c>
       <c r="Y20" t="s">
         <v>18</v>
@@ -6326,23 +6328,23 @@
       </c>
       <c r="I22" s="8">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!I$15,ar6_r10!$M$2:$M$999,Veda!$E22)</f>
-        <v>71.48</v>
+        <v>241.69</v>
       </c>
       <c r="J22" s="8">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!J$15,ar6_r10!$M$2:$M$999,Veda!$E22)</f>
-        <v>104.42</v>
+        <v>339.03</v>
       </c>
       <c r="K22" s="8">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!K$15,ar6_r10!$M$2:$M$999,Veda!$E22)</f>
-        <v>134.85</v>
+        <v>410.28</v>
       </c>
       <c r="L22" s="8">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!L$15,ar6_r10!$M$2:$M$999,Veda!$E22)</f>
-        <v>178.1</v>
+        <v>494.2</v>
       </c>
       <c r="M22" s="8">
         <f>SUMIFS(ar6_r10!$F$2:$F$999,ar6_r10!$A$2:$A$999,Veda!$C$5,ar6_r10!$C$2:$C$999,Veda!M$15,ar6_r10!$M$2:$M$999,Veda!$E22)</f>
-        <v>209.45</v>
+        <v>635.42999999999995</v>
       </c>
       <c r="Q22" t="s">
         <v>29</v>
@@ -6352,23 +6354,23 @@
       </c>
       <c r="T22" s="11">
         <f>I22/1000</f>
-        <v>7.1480000000000002E-2</v>
+        <v>0.24168999999999999</v>
       </c>
       <c r="U22" s="11">
         <f>J22/1000</f>
-        <v>0.10442</v>
+        <v>0.33903</v>
       </c>
       <c r="V22" s="11">
         <f>K22/1000</f>
-        <v>0.13485</v>
+        <v>0.41027999999999998</v>
       </c>
       <c r="W22" s="11">
         <f>L22/1000</f>
-        <v>0.17809999999999998</v>
+        <v>0.49419999999999997</v>
       </c>
       <c r="X22" s="11">
         <f>M22/1000</f>
-        <v>0.20945</v>
+        <v>0.63542999999999994</v>
       </c>
       <c r="Y22" t="s">
         <v>30</v>
@@ -7310,7 +7312,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D3AADB-9A32-40E9-8F4D-C4BF39898AB4}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -7400,7 +7404,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -8126,7 +8132,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M360"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -22439,7 +22447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0ACD839-B60C-4CDA-B632-BF39C559A5EF}">
   <dimension ref="B10:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>

</xml_diff>